<commit_message>
Cambiar guardar nombres de equipo por Objetos de Equipo
En las listas de partidos contra quien ha gandao y perdido, en vezs de guardar el nombre, guardo el objeto, para poder entrar y revisarlo cuando quiera y lo que quiera.
</commit_message>
<xml_diff>
--- a/Bets.xlsx
+++ b/Bets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\Desktop\Projects\Python Programs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\Desktop\Projects\Python Programs\Bets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DE401E-6902-4BDC-AA29-A88160ED3CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F6C441-58F5-475F-854D-8388C888B752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -658,13 +658,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:U21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
     <col min="5" max="24" width="9.7109375" customWidth="1"/>
     <col min="27" max="27" width="23.28515625" customWidth="1"/>
@@ -1605,7 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B89604-6B94-4E15-A8D0-6DC6452889EC}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Method Strenght and Weakness Done
Method is working fine and i will start creating ohter methods and statistics
</commit_message>
<xml_diff>
--- a/Bets.xlsx
+++ b/Bets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domin\Desktop\Projects\Python Programs\Bets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F6C441-58F5-475F-854D-8388C888B752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C287FC61-FA89-43A1-8151-76C8E51135C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4695" yWindow="2115" windowWidth="14400" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="25">
   <si>
     <t>Barcelona</t>
   </si>
@@ -126,7 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,19 +134,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3C4043"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -331,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,7 +369,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -656,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF35"/>
+  <dimension ref="A1:BF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18:O19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,11 +759,11 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
@@ -770,14 +782,8 @@
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="T2" s="1"/>
       <c r="U2" s="2"/>
-      <c r="V2">
-        <f>COUNTIF(B2:U2,"G")</f>
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -796,23 +802,19 @@
         <v>21</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="R3" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="2"/>
-      <c r="V3">
-        <f t="shared" ref="V3:V21" si="0">COUNTIF(B3:U3,"G")</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -829,27 +831,21 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="2"/>
-      <c r="V4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -869,8 +865,10 @@
         <v>21</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="N5" s="1" t="s">
         <v>21</v>
       </c>
@@ -881,10 +879,6 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="2"/>
-      <c r="V5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -906,9 +900,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
         <v>21</v>
       </c>
@@ -916,47 +908,39 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
+      <c r="T6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="U6" s="2"/>
-      <c r="V6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    </row>
+    <row r="7" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="2"/>
-      <c r="V7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="15"/>
     </row>
     <row r="8" spans="1:58" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -966,9 +950,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
         <v>20</v>
@@ -979,7 +961,9 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="O8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -988,58 +972,53 @@
         <v>21</v>
       </c>
       <c r="U8" s="2"/>
-      <c r="V8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+      <c r="V8"/>
       <c r="Y8" s="10"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" s="1"/>
-      <c r="U9" s="2"/>
-      <c r="V9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="15"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="17"/>
+      <c r="AF9" s="17"/>
+      <c r="AG9" s="17"/>
+      <c r="AH9" s="17"/>
+      <c r="AI9" s="17"/>
+      <c r="AJ9" s="17"/>
+      <c r="AK9" s="17"/>
+      <c r="AL9" s="17"/>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1056,9 +1035,7 @@
       <c r="J10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1069,10 +1046,6 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="2"/>
-      <c r="V10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
@@ -1108,50 +1081,44 @@
       <c r="BE10" s="3"/>
       <c r="BF10" s="3"/>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="2"/>
-      <c r="V11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="15"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -1174,19 +1141,13 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="Q12" s="1"/>
       <c r="R12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="2"/>
-      <c r="V12">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
@@ -1222,58 +1183,48 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="V13">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="U13" s="2"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="2"/>
-      <c r="V14">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="15"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -1303,10 +1254,6 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="2"/>
-      <c r="V15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
@@ -1339,61 +1286,51 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="T16" s="1"/>
       <c r="U16" s="2"/>
-      <c r="V16">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="V17">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" s="13"/>
+      <c r="U17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -1421,10 +1358,6 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="2"/>
-      <c r="V18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
@@ -1447,24 +1380,20 @@
       <c r="K19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="R19" s="1"/>
       <c r="S19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="2"/>
-      <c r="V19">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
@@ -1497,10 +1426,6 @@
         <v>20</v>
       </c>
       <c r="U20" s="2"/>
-      <c r="V20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
@@ -1535,10 +1460,6 @@
       <c r="U21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
@@ -1566,36 +1487,12 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="3"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="3"/>
-    </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AA28" s="3"/>
-      <c r="AB28" s="3"/>
-      <c r="AC28" s="3"/>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
-      <c r="N35" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1655,7 +1552,7 @@
       <c r="U1" s="9"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1684,7 +1581,7 @@
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1711,7 +1608,7 @@
       <c r="U3" s="2"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
@@ -1736,7 +1633,7 @@
       <c r="U4" s="2"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1759,7 +1656,7 @@
       <c r="U5" s="2"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1"/>
@@ -1784,7 +1681,7 @@
       <c r="U6" s="2"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>

</xml_diff>